<commit_message>
Add HTTPS support, acme service, and nginx certs
Enable HTTPS for the frontend and add ACME-based certificate management. Adds frontend/certs/README.md with mkcert and acme.sh instructions, updates nginx.conf to serve ACME challenges, redirect HTTP->HTTPS, provide /healthz, and enforce TLS + security headers. docker-compose.yml changed to expose 80/443 for the frontend, mount certs and ACME webroot, add an acme service, and adjust VITE_API_URL and backend exposure. Frontend Dockerfile updated to expose 80/443, use /healthz for health checks, and reload nginx periodically to pick up renewed certs. .gitignore updated to ignore local cert files and acme state. Also small docs and artifacts updates: INSTALLATION.md references docker compose and HTTPS options, backend notebook output updated, and results/stat.xlsx changed.
</commit_message>
<xml_diff>
--- a/results/stat.xlsx
+++ b/results/stat.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anoureldin\Desktop\TSP\semi-supervised-labeling-framework\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C92E2B-6AE6-471F-8E2C-E498C35B77A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D103A32-C6BE-4F85-8A18-EA81B4F09EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="question overlap" sheetId="6" r:id="rId1"/>
     <sheet name="stat label" sheetId="1" r:id="rId2"/>
-    <sheet name="eval labels" sheetId="2" r:id="rId3"/>
-    <sheet name="stat questions" sheetId="5" r:id="rId4"/>
+    <sheet name="LLM-as-Judge eval labels" sheetId="2" r:id="rId3"/>
+    <sheet name="Human eval labels" sheetId="7" r:id="rId4"/>
+    <sheet name="LLM-as-Judge eval questions" sheetId="5" r:id="rId5"/>
+    <sheet name="Human eval questions" sheetId="8" r:id="rId6"/>
+    <sheet name="Human eval labels details" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="102">
   <si>
     <t>method</t>
   </si>
@@ -292,13 +295,64 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>source  ChatGPT</t>
+  </si>
+  <si>
+    <t>ISO/IEC 27002</t>
+  </si>
+  <si>
+    <t>ISO/IEC 27017</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>iso 27002 from iso 27002</t>
+  </si>
+  <si>
+    <t>Completeness</t>
+  </si>
+  <si>
+    <t>KNN (derived from ISO/IEC 27017)</t>
+  </si>
+  <si>
+    <t>Generalizability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +378,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Docs-Roboto"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Docs-Roboto"/>
     </font>
   </fonts>
   <fills count="3">
@@ -352,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -375,9 +440,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -389,6 +451,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -670,15 +752,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58DF0B6-02D2-46DA-860D-19051A161656}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>31</v>
       </c>
@@ -698,7 +780,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -721,7 +803,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -744,7 +826,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -767,7 +849,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -790,7 +872,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -813,7 +895,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -834,6 +916,11 @@
       </c>
       <c r="G7" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +936,7 @@
       <selection activeCell="I22" sqref="I22:I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" style="1" customWidth="1"/>
@@ -863,7 +950,7 @@
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -921,7 +1008,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
         <v>36</v>
       </c>
@@ -950,7 +1037,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
@@ -979,7 +1066,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1008,7 +1095,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -1037,7 +1124,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="5" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -1066,7 +1153,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1095,7 +1182,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -1124,7 +1211,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="7" t="s">
         <v>33</v>
       </c>
@@ -1153,7 +1240,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
@@ -1182,7 +1269,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -1211,7 +1298,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="5" customFormat="1">
       <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
@@ -1240,7 +1327,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1248,7 +1335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1256,7 +1343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1264,7 +1351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1272,7 +1359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="7" customFormat="1">
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
@@ -1280,7 +1367,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1384,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1314,7 +1401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1331,7 +1418,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1348,7 +1435,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" s="7" customFormat="1">
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
@@ -1365,7 +1452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1379,7 +1466,7 @@
         <v>3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -1387,7 +1474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
@@ -1395,7 +1482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1403,7 +1490,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="7" customFormat="1">
       <c r="A32" s="7" t="s">
         <v>16</v>
       </c>
@@ -1411,7 +1498,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -1425,7 +1512,7 @@
         <v>3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -1433,7 +1520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
@@ -1441,7 +1528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -1449,7 +1536,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" s="7" customFormat="1">
       <c r="A38" s="7" t="s">
         <v>17</v>
       </c>
@@ -1457,7 +1544,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>18</v>
       </c>
@@ -1471,7 +1558,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>18</v>
       </c>
@@ -1479,7 +1566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>18</v>
       </c>
@@ -1487,7 +1574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>18</v>
       </c>
@@ -1495,7 +1582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" s="7" customFormat="1">
       <c r="A44" s="7" t="s">
         <v>18</v>
       </c>
@@ -1503,8 +1590,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" s="7" customFormat="1"/>
+    <row r="46" spans="1:5" s="7" customFormat="1">
       <c r="A46" s="7" t="s">
         <v>41</v>
       </c>
@@ -1512,7 +1599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" s="7" customFormat="1">
       <c r="A47" s="7" t="s">
         <v>41</v>
       </c>
@@ -1520,7 +1607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" s="7" customFormat="1">
       <c r="A48" s="7" t="s">
         <v>41</v>
       </c>
@@ -1528,7 +1615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" s="7" customFormat="1">
       <c r="A49" s="7" t="s">
         <v>41</v>
       </c>
@@ -1536,7 +1623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" s="7" customFormat="1">
       <c r="A50" s="7" t="s">
         <v>41</v>
       </c>
@@ -1544,7 +1631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
         <v>20</v>
       </c>
@@ -1561,7 +1648,7 @@
         <v>5.8999999999999998E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
         <v>20</v>
       </c>
@@ -1578,7 +1665,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
         <v>20</v>
       </c>
@@ -1595,7 +1682,7 @@
         <v>4.1E-5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
         <v>20</v>
       </c>
@@ -1612,7 +1699,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
         <v>20</v>
       </c>
@@ -1629,7 +1716,7 @@
         <v>4.3999999999999999E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5">
       <c r="A57" s="6" t="s">
         <v>20</v>
       </c>
@@ -1657,10 +1744,10 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -1678,32 +1765,32 @@
     <col min="14" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="8" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="10"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="13"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="7" t="s">
         <v>23</v>
       </c>
@@ -1713,7 +1800,7 @@
       <c r="E2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
@@ -1723,7 +1810,7 @@
       <c r="I2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="10"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
@@ -1734,11 +1821,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="1">
@@ -1750,7 +1837,7 @@
       <c r="E3" s="1">
         <v>4.5599999999999996</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G3" s="1">
@@ -1762,7 +1849,7 @@
       <c r="I3" s="1">
         <v>4.78</v>
       </c>
-      <c r="J3" s="10"/>
+      <c r="J3" s="9"/>
       <c r="K3" s="1">
         <f>C3-G3</f>
         <v>-1.46</v>
@@ -1776,14 +1863,14 @@
         <v>-0.22000000000000064</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>3.3</v>
       </c>
       <c r="D4" s="1">
@@ -1792,7 +1879,7 @@
       <c r="E4" s="1">
         <v>4.68</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="1">
@@ -1804,7 +1891,7 @@
       <c r="I4" s="1">
         <v>4.93</v>
       </c>
-      <c r="J4" s="10"/>
+      <c r="J4" s="9"/>
       <c r="K4" s="7">
         <f t="shared" ref="K4:K8" si="1">C4-G4</f>
         <v>-1.6000000000000005</v>
@@ -1818,11 +1905,11 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="1">
@@ -1834,7 +1921,7 @@
       <c r="E5" s="1">
         <v>4.75</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="1">
@@ -1846,7 +1933,7 @@
       <c r="I5" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J5" s="10"/>
+      <c r="J5" s="9"/>
       <c r="K5" s="7">
         <f t="shared" si="1"/>
         <v>-0.91000000000000014</v>
@@ -1860,11 +1947,11 @@
         <v>-0.15000000000000036</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="1">
@@ -1876,7 +1963,7 @@
       <c r="E6" s="1">
         <v>4.72</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="1">
@@ -1888,7 +1975,7 @@
       <c r="I6" s="1">
         <v>4.63</v>
       </c>
-      <c r="J6" s="10"/>
+      <c r="J6" s="9"/>
       <c r="K6" s="7">
         <f t="shared" si="1"/>
         <v>-1.1300000000000003</v>
@@ -1902,11 +1989,11 @@
         <v>8.9999999999999858E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="1">
@@ -1918,7 +2005,7 @@
       <c r="E7" s="1">
         <v>4.6900000000000004</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G7" s="1">
@@ -1930,7 +2017,7 @@
       <c r="I7" s="1">
         <v>4.88</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="9"/>
       <c r="K7" s="7">
         <f t="shared" si="1"/>
         <v>-1.5</v>
@@ -1944,11 +2031,11 @@
         <v>-0.1899999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="1">
@@ -1960,7 +2047,7 @@
       <c r="E8" s="1">
         <v>4.7300000000000004</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G8" s="1">
@@ -1972,7 +2059,7 @@
       <c r="I8" s="1">
         <v>4.8899999999999997</v>
       </c>
-      <c r="J8" s="10"/>
+      <c r="J8" s="9"/>
       <c r="K8" s="7">
         <f t="shared" si="1"/>
         <v>-0.94999999999999973</v>
@@ -1986,11 +2073,11 @@
         <v>-0.15999999999999925</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="1">
@@ -2002,7 +2089,7 @@
       <c r="E12" s="1">
         <v>4.6100000000000003</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="1">
@@ -2027,11 +2114,11 @@
         <v>-0.29999999999999982</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="1">
@@ -2043,7 +2130,7 @@
       <c r="E13" s="1">
         <v>4.58</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G13" s="1">
@@ -2068,11 +2155,11 @@
         <v>-0.33000000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="1">
@@ -2084,7 +2171,7 @@
       <c r="E14" s="1">
         <v>4.79</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G14" s="1">
@@ -2109,11 +2196,11 @@
         <v>-8.0000000000000071E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="1">
@@ -2125,7 +2212,7 @@
       <c r="E15" s="1">
         <v>4.8600000000000003</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="1">
@@ -2150,11 +2237,11 @@
         <v>1.0000000000000675E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="1">
@@ -2166,7 +2253,7 @@
       <c r="E16" s="1">
         <v>4.78</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="1">
@@ -2191,9 +2278,9 @@
         <v>-9.9999999999999645E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="7"/>
-      <c r="B17" s="12"/>
+      <c r="B17" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2208,14 +2295,181 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB83A05-913C-4551-8F73-E52EE6F57840}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="13"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="12">
+        <f>C3-H3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="12">
+        <f t="shared" ref="N3:P3" si="0">D3-I3</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="12">
+        <f>C4-H4</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="12">
+        <f t="shared" ref="N4" si="1">D4-I4</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="12">
+        <f t="shared" ref="O4" si="2">E4-J4</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="12">
+        <f t="shared" ref="P4" si="3">F4-K4</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="M1:P1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AD7ABB-C516-4DB3-B325-481AF92A7F95}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.44140625" bestFit="1" customWidth="1"/>
@@ -2225,7 +2479,7 @@
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2242,7 +2496,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2259,7 +2513,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2276,7 +2530,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2293,7 +2547,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2310,7 +2564,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2327,7 +2581,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2344,7 +2598,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2361,7 +2615,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -2378,7 +2632,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -2399,4 +2653,352 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7750330D-7268-4063-9DA5-18FFA075A224}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E4A3B1-2F83-4EAD-94AD-63F8452841B9}">
+  <dimension ref="A1:AX6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.33203125" customWidth="1"/>
+    <col min="15" max="23" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="4.33203125" customWidth="1"/>
+    <col min="27" max="35" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="4.109375" customWidth="1"/>
+    <col min="38" max="38" width="3.5546875" customWidth="1"/>
+    <col min="39" max="47" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="3.77734375" customWidth="1"/>
+    <col min="50" max="50" width="4.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:50">
+      <c r="C1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="16"/>
+      <c r="AX1" s="18"/>
+    </row>
+    <row r="2" spans="1:50">
+      <c r="C2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" s="15"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="X2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD2" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI2" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP2" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU2" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX2" s="18"/>
+    </row>
+    <row r="3" spans="1:50">
+      <c r="A3" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="e">
+        <f>AVERAGE(C3:L3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N3" s="18"/>
+      <c r="Y3" t="e">
+        <f>AVERAGE(O3:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Z3" s="18"/>
+      <c r="AK3" t="e">
+        <f>AVERAGE(AA3:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AL3" s="18"/>
+      <c r="AW3" t="e">
+        <f>AVERAGE(AM3:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AX3" s="18"/>
+    </row>
+    <row r="4" spans="1:50">
+      <c r="A4" s="17"/>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="e">
+        <f t="shared" ref="M4:M6" si="0">AVERAGE(C4:L4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N4" s="18"/>
+      <c r="Y4" t="e">
+        <f>AVERAGE(O4:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Z4" s="18"/>
+      <c r="AK4" t="e">
+        <f>AVERAGE(AA4:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AL4" s="18"/>
+      <c r="AW4" t="e">
+        <f>AVERAGE(AM4:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AX4" s="18"/>
+    </row>
+    <row r="5" spans="1:50">
+      <c r="A5" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N5" s="18"/>
+      <c r="Y5" t="e">
+        <f>AVERAGE(O5:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Z5" s="18"/>
+      <c r="AK5" t="e">
+        <f>AVERAGE(AA5:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AL5" s="18"/>
+      <c r="AW5" t="e">
+        <f>AVERAGE(AM5:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AX5" s="18"/>
+    </row>
+    <row r="6" spans="1:50">
+      <c r="A6" s="17"/>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="M6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="18"/>
+      <c r="Y6" t="e">
+        <f>AVERAGE(O6:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Z6" s="18"/>
+      <c r="AK6" t="e">
+        <f>AVERAGE(AA6:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AL6" s="18"/>
+      <c r="AW6" t="e">
+        <f>AVERAGE(AM6:X5X3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AX6" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="AM1:AV1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="O1:X1"/>
+    <mergeCell ref="AA1:AJ1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add evaluation notebook; update Docker & results
Add a combined_evaluation.ipynb (computes main and query-evaluation metrics and writes final_results.xlsx) and add final_results.xlsx. Update backend Dockerfile to use python:3.11-slim-bookworm and install scikit-cmeans with --no-build-isolation. Update frontend Dockerfile to expose a build ARG/ENV VITE_API_URL and adjust docker-compose.yml to pass the build arg and remove the runtime VITE_API_URL env; also add a network setting for the backend service. Rename one similarity CSV and update similarity/result CSV and stat.xlsx binary to include refreshed results.
</commit_message>
<xml_diff>
--- a/results/stat.xlsx
+++ b/results/stat.xlsx
@@ -8,18 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anoureldin\Desktop\TSP\semi-supervised-labeling-framework\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D103A32-C6BE-4F85-8A18-EA81B4F09EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348FDDEB-636B-4B9D-9501-487FFBC72A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="question overlap" sheetId="6" r:id="rId1"/>
     <sheet name="stat label" sheetId="1" r:id="rId2"/>
     <sheet name="LLM-as-Judge eval labels" sheetId="2" r:id="rId3"/>
     <sheet name="Human eval labels" sheetId="7" r:id="rId4"/>
-    <sheet name="LLM-as-Judge eval questions" sheetId="5" r:id="rId5"/>
-    <sheet name="Human eval questions" sheetId="8" r:id="rId6"/>
-    <sheet name="Human eval labels details" sheetId="9" r:id="rId7"/>
+    <sheet name="eval questions" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="92">
   <si>
     <t>method</t>
   </si>
@@ -285,9 +283,6 @@
     <t>6,23 s</t>
   </si>
   <si>
-    <t>score</t>
-  </si>
-  <si>
     <t>Backup Frequency &amp; Retention &amp; Monitoring &amp; Incident Response</t>
   </si>
   <si>
@@ -303,56 +298,29 @@
     <t>ISO/IEC 27002</t>
   </si>
   <si>
-    <t>ISO/IEC 27017</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>Q7</t>
-  </si>
-  <si>
-    <t>Q8</t>
-  </si>
-  <si>
-    <t>Q9</t>
-  </si>
-  <si>
-    <t>Q10</t>
-  </si>
-  <si>
-    <t>iso 27002 from iso 27002</t>
-  </si>
-  <si>
-    <t>Completeness</t>
-  </si>
-  <si>
-    <t>KNN (derived from ISO/IEC 27017)</t>
-  </si>
-  <si>
-    <t>Generalizability</t>
+    <t>iso 27017 from iso 27002</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLM-as-Judge </t>
+  </si>
+  <si>
+    <t>score/100</t>
+  </si>
+  <si>
+    <t>score/5</t>
+  </si>
+  <si>
+    <t>Human eval</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,17 +346,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Docs-Roboto"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Docs-Roboto"/>
     </font>
   </fonts>
   <fills count="3">
@@ -417,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -458,19 +415,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,9 +704,9 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>31</v>
       </c>
@@ -780,7 +726,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -803,7 +749,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -826,7 +772,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -849,7 +795,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -872,7 +818,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -895,7 +841,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -918,9 +864,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -932,11 +878,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22:I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I9:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" style="1" customWidth="1"/>
@@ -950,7 +896,7 @@
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -979,7 +925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -1008,7 +954,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>36</v>
       </c>
@@ -1037,7 +983,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
@@ -1066,7 +1012,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1095,7 +1041,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -1124,7 +1070,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1">
+    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -1153,7 +1099,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1182,7 +1128,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -1211,7 +1157,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>33</v>
       </c>
@@ -1240,7 +1186,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
@@ -1269,7 +1215,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -1298,7 +1244,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="5" customFormat="1">
+    <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
@@ -1327,7 +1273,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1335,7 +1281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1343,7 +1289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1351,7 +1297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1359,7 +1305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="7" customFormat="1">
+    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
@@ -1367,7 +1313,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -1384,7 +1330,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1401,7 +1347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1418,7 +1364,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1435,7 +1381,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="7" customFormat="1">
+    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1466,7 +1412,7 @@
         <v>3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -1474,7 +1420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
@@ -1482,7 +1428,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1490,7 +1436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="7" customFormat="1">
+    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>16</v>
       </c>
@@ -1498,7 +1444,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -1512,7 +1458,7 @@
         <v>3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -1520,7 +1466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
@@ -1528,7 +1474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -1536,7 +1482,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="7" customFormat="1">
+    <row r="38" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>17</v>
       </c>
@@ -1544,7 +1490,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>18</v>
       </c>
@@ -1558,7 +1504,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>18</v>
       </c>
@@ -1566,7 +1512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>18</v>
       </c>
@@ -1574,7 +1520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>18</v>
       </c>
@@ -1582,7 +1528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="7" customFormat="1">
+    <row r="44" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>18</v>
       </c>
@@ -1590,8 +1536,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="7" customFormat="1"/>
-    <row r="46" spans="1:5" s="7" customFormat="1">
+    <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>41</v>
       </c>
@@ -1599,7 +1545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="7" customFormat="1">
+    <row r="47" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>41</v>
       </c>
@@ -1607,7 +1553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="7" customFormat="1">
+    <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>41</v>
       </c>
@@ -1615,7 +1561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="7" customFormat="1">
+    <row r="49" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>41</v>
       </c>
@@ -1623,7 +1569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="7" customFormat="1">
+    <row r="50" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>41</v>
       </c>
@@ -1631,7 +1577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>20</v>
       </c>
@@ -1648,7 +1594,7 @@
         <v>5.8999999999999998E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>20</v>
       </c>
@@ -1665,7 +1611,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1628,7 @@
         <v>4.1E-5</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>20</v>
       </c>
@@ -1699,7 +1645,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>20</v>
       </c>
@@ -1716,7 +1662,7 @@
         <v>4.3999999999999999E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>20</v>
       </c>
@@ -1744,10 +1690,10 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C12" sqref="C12:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -1765,31 +1711,31 @@
     <col min="14" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="8"/>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="13"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
       <c r="B2" s="9"/>
       <c r="C2" s="7" t="s">
         <v>23</v>
@@ -1821,7 +1767,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -1832,10 +1778,10 @@
         <v>3.29</v>
       </c>
       <c r="D3" s="1">
-        <v>4.03</v>
+        <v>4.13</v>
       </c>
       <c r="E3" s="1">
-        <v>4.5599999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>33</v>
@@ -1844,7 +1790,7 @@
         <v>4.75</v>
       </c>
       <c r="H3" s="1">
-        <v>4.42</v>
+        <v>4.32</v>
       </c>
       <c r="I3" s="1">
         <v>4.78</v>
@@ -1856,14 +1802,14 @@
       </c>
       <c r="L3" s="7">
         <f t="shared" ref="L3:M3" si="0">D3-H3</f>
-        <v>-0.38999999999999968</v>
+        <v>-0.19000000000000039</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="0"/>
-        <v>-0.22000000000000064</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>-8.0000000000000071E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1874,7 +1820,7 @@
         <v>3.3</v>
       </c>
       <c r="D4" s="1">
-        <v>4.12</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="E4" s="1">
         <v>4.68</v>
@@ -1886,7 +1832,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="H4" s="1">
-        <v>4.6900000000000004</v>
+        <v>4.49</v>
       </c>
       <c r="I4" s="1">
         <v>4.93</v>
@@ -1898,14 +1844,14 @@
       </c>
       <c r="L4" s="7">
         <f t="shared" ref="L4:L8" si="2">D4-H4</f>
-        <v>-0.57000000000000028</v>
+        <v>2.9999999999999361E-2</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" ref="M4:M8" si="3">E4-I4</f>
         <v>-0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1928,7 +1874,7 @@
         <v>4.8600000000000003</v>
       </c>
       <c r="H5" s="1">
-        <v>4.62</v>
+        <v>4.42</v>
       </c>
       <c r="I5" s="1">
         <v>4.9000000000000004</v>
@@ -1940,14 +1886,14 @@
       </c>
       <c r="L5" s="7">
         <f t="shared" si="2"/>
-        <v>-0.28000000000000025</v>
+        <v>-8.0000000000000071E-2</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="3"/>
         <v>-0.15000000000000036</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1958,7 +1904,7 @@
         <v>3.48</v>
       </c>
       <c r="D6" s="1">
-        <v>4.16</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="E6" s="1">
         <v>4.72</v>
@@ -1982,14 +1928,14 @@
       </c>
       <c r="L6" s="7">
         <f t="shared" si="2"/>
-        <v>-0.1899999999999995</v>
+        <v>1.0000000000000675E-2</v>
       </c>
       <c r="M6" s="7">
         <f t="shared" si="3"/>
         <v>8.9999999999999858E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2000,7 +1946,7 @@
         <v>3.33</v>
       </c>
       <c r="D7" s="1">
-        <v>4.1100000000000003</v>
+        <v>4.25</v>
       </c>
       <c r="E7" s="1">
         <v>4.6900000000000004</v>
@@ -2012,7 +1958,7 @@
         <v>4.83</v>
       </c>
       <c r="H7" s="1">
-        <v>4.5199999999999996</v>
+        <v>4.32</v>
       </c>
       <c r="I7" s="1">
         <v>4.88</v>
@@ -2024,14 +1970,14 @@
       </c>
       <c r="L7" s="7">
         <f t="shared" si="2"/>
-        <v>-0.40999999999999925</v>
+        <v>-7.0000000000000284E-2</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="3"/>
         <v>-0.1899999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
@@ -2042,7 +1988,7 @@
         <v>3.89</v>
       </c>
       <c r="D8" s="1">
-        <v>4.25</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="E8" s="1">
         <v>4.7300000000000004</v>
@@ -2054,7 +2000,7 @@
         <v>4.84</v>
       </c>
       <c r="H8" s="1">
-        <v>4.58</v>
+        <v>4.38</v>
       </c>
       <c r="I8" s="1">
         <v>4.8899999999999997</v>
@@ -2066,14 +2012,14 @@
       </c>
       <c r="L8" s="7">
         <f t="shared" si="2"/>
-        <v>-0.33000000000000007</v>
+        <v>-3.0000000000000249E-2</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="3"/>
         <v>-0.15999999999999925</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
@@ -2114,7 +2060,7 @@
         <v>-0.29999999999999982</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>44</v>
       </c>
@@ -2155,7 +2101,7 @@
         <v>-0.33000000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>45</v>
       </c>
@@ -2196,7 +2142,7 @@
         <v>-8.0000000000000071E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>46</v>
       </c>
@@ -2237,7 +2183,7 @@
         <v>1.0000000000000675E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>47</v>
       </c>
@@ -2278,7 +2224,7 @@
         <v>-9.9999999999999645E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11"/>
     </row>
@@ -2296,164 +2242,165 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB83A05-913C-4551-8F73-E52EE6F57840}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="13" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="13"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
       <c r="B2" s="9"/>
       <c r="C2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>99</v>
+      <c r="D2" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="12" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="9" t="s">
+      <c r="C3" s="13">
+        <v>4.1920000000000002</v>
+      </c>
+      <c r="D3" s="13">
+        <v>4.2080000000000002</v>
+      </c>
+      <c r="E3" s="12">
+        <v>4.0119999999999996</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="9"/>
+      <c r="G3" s="12">
+        <v>4.3680000000000003</v>
+      </c>
+      <c r="H3" s="12">
+        <v>3.944</v>
+      </c>
+      <c r="I3" s="12">
+        <v>4.1479999999999997</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="12">
+        <f>C3-G3</f>
+        <v>-0.17600000000000016</v>
+      </c>
+      <c r="L3" s="12">
+        <f>D3-H3</f>
+        <v>0.26400000000000023</v>
+      </c>
       <c r="M3" s="12">
-        <f>C3-H3</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="12">
-        <f t="shared" ref="N3:P3" si="0">D3-I3</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <f>E3-I3</f>
+        <v>-0.13600000000000012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="9" t="s">
+      <c r="C4" s="12">
+        <v>3.7440000000000002</v>
+      </c>
+      <c r="D4" s="12">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E4" s="12">
+        <v>3.8319999999999999</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="9"/>
+      <c r="G4" s="12">
+        <v>4.5279999999999996</v>
+      </c>
+      <c r="H4" s="12">
+        <v>3.9279999999999999</v>
+      </c>
+      <c r="I4" s="12">
+        <v>4.2960000000000003</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="12">
+        <f>C4-G4</f>
+        <v>-0.78399999999999936</v>
+      </c>
+      <c r="L4" s="12">
+        <f>D4-H4</f>
+        <v>0.17199999999999971</v>
+      </c>
       <c r="M4" s="12">
-        <f>C4-H4</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="12">
-        <f t="shared" ref="N4" si="1">D4-I4</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="12">
-        <f t="shared" ref="O4" si="2">E4-J4</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="12">
-        <f t="shared" ref="P4" si="3">F4-K4</f>
-        <v>0</v>
+        <f>E4-I4</f>
+        <v>-0.46400000000000041</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2463,13 +2410,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AD7ABB-C516-4DB3-B325-481AF92A7F95}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.44140625" bestFit="1" customWidth="1"/>
@@ -2479,7 +2426,7 @@
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2493,10 +2440,13 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2512,8 +2462,11 @@
       <c r="E2">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2524,13 +2477,16 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2546,8 +2502,11 @@
       <c r="E4">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2563,8 +2522,11 @@
       <c r="E5">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2575,13 +2537,16 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2597,13 +2562,16 @@
       <c r="E7">
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
@@ -2614,30 +2582,36 @@
       <c r="E8">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -2647,358 +2621,73 @@
       </c>
       <c r="E10">
         <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14">
+        <v>3.95</v>
+      </c>
+      <c r="F14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15">
+        <v>3.24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7750330D-7268-4063-9DA5-18FFA075A224}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E4A3B1-2F83-4EAD-94AD-63F8452841B9}">
-  <dimension ref="A1:AX6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.33203125" customWidth="1"/>
-    <col min="15" max="23" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="4.33203125" customWidth="1"/>
-    <col min="27" max="35" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="4.109375" customWidth="1"/>
-    <col min="38" max="38" width="3.5546875" customWidth="1"/>
-    <col min="39" max="47" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="3.77734375" customWidth="1"/>
-    <col min="50" max="50" width="4.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:50">
-      <c r="C1" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
-      <c r="AX1" s="18"/>
-    </row>
-    <row r="2" spans="1:50">
-      <c r="C2" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="V2" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="X2" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC2" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD2" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF2" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG2" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH2" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="AI2" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ2" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO2" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="AP2" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AR2" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="AS2" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AT2" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="AU2" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="AV2" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="AX2" s="18"/>
-    </row>
-    <row r="3" spans="1:50">
-      <c r="A3" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" t="e">
-        <f>AVERAGE(C3:L3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N3" s="18"/>
-      <c r="Y3" t="e">
-        <f>AVERAGE(O3:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Z3" s="18"/>
-      <c r="AK3" t="e">
-        <f>AVERAGE(AA3:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="AL3" s="18"/>
-      <c r="AW3" t="e">
-        <f>AVERAGE(AM3:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="AX3" s="18"/>
-    </row>
-    <row r="4" spans="1:50">
-      <c r="A4" s="17"/>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" t="e">
-        <f t="shared" ref="M4:M6" si="0">AVERAGE(C4:L4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N4" s="18"/>
-      <c r="Y4" t="e">
-        <f>AVERAGE(O4:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Z4" s="18"/>
-      <c r="AK4" t="e">
-        <f>AVERAGE(AA4:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="AL4" s="18"/>
-      <c r="AW4" t="e">
-        <f>AVERAGE(AM4:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="AX4" s="18"/>
-    </row>
-    <row r="5" spans="1:50">
-      <c r="A5" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N5" s="18"/>
-      <c r="Y5" t="e">
-        <f>AVERAGE(O5:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Z5" s="18"/>
-      <c r="AK5" t="e">
-        <f>AVERAGE(AA5:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="AL5" s="18"/>
-      <c r="AW5" t="e">
-        <f>AVERAGE(AM5:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="AX5" s="18"/>
-    </row>
-    <row r="6" spans="1:50">
-      <c r="A6" s="17"/>
-      <c r="B6" t="s">
-        <v>100</v>
-      </c>
-      <c r="M6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N6" s="18"/>
-      <c r="Y6" t="e">
-        <f>AVERAGE(O6:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Z6" s="18"/>
-      <c r="AK6" t="e">
-        <f>AVERAGE(AA6:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="AL6" s="18"/>
-      <c r="AW6" t="e">
-        <f>AVERAGE(AM6:X5X3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="AX6" s="18"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="AM1:AV1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="O1:X1"/>
-    <mergeCell ref="AA1:AJ1"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>